<commit_message>
Used a normal approximation
</commit_message>
<xml_diff>
--- a/Financial_Modeling_SimTrade_VaR_calculation.xlsx
+++ b/Financial_Modeling_SimTrade_VaR_calculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{55E31D62-73E6-4870-AB99-EB59BE69401E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0D8CAFBC-65BC-48B1-B58E-14939D69006C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="32" uniqueCount="23">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="34" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>Underflow</t>
+  </si>
+  <si>
+    <t>Std Dev</t>
   </si>
 </sst>
 </file>
@@ -13928,8 +13931,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{802F29F9-E7D8-418D-8598-248BD26C39A9}">
   <dimension ref="A1:V493"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E18" workbookViewId="0">
-      <selection activeCell="R33" sqref="R33"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -14865,8 +14868,15 @@
       <c r="E32" s="32">
         <v>-2.0066766142794954</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="O32" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P32" s="32">
+        <f>AVERAGE(_xlfn.ANCHORARRAY(E3))</f>
+        <v>4.3929319156568843E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="32">
         <v>43871</v>
       </c>
@@ -14880,8 +14890,15 @@
       <c r="E33" s="32">
         <v>-1.9370244624565454</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="O33" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="P33" s="32">
+        <f>_xlfn.STDEV.P(_xlfn.ANCHORARRAY(E3))</f>
+        <v>1.5715646872301317</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="32">
         <v>43872</v>
       </c>
@@ -14896,7 +14913,7 @@
         <v>-1.9048243331566181</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="32">
         <v>43873</v>
       </c>
@@ -14910,8 +14927,15 @@
       <c r="E35" s="32">
         <v>-1.8992154718224015</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="O35" s="35">
+        <v>0.01</v>
+      </c>
+      <c r="P35" s="32">
+        <f>_xlfn.NORM.INV(O35,$P$32,$P$33)</f>
+        <v>-3.6120768498989064</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="32">
         <v>43874</v>
       </c>
@@ -14925,8 +14949,15 @@
       <c r="E36" s="32">
         <v>-1.8571919569897599</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="O36" s="35">
+        <v>0.05</v>
+      </c>
+      <c r="P36" s="32">
+        <f>_xlfn.NORM.INV(O36,$P$32,$P$33)</f>
+        <v>-2.5410645566227696</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="32">
         <v>43875</v>
       </c>
@@ -14941,7 +14972,7 @@
         <v>-1.7744565941854906</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="32">
         <v>43878</v>
       </c>
@@ -14956,7 +14987,7 @@
         <v>-1.7408915575824335</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="32">
         <v>43879</v>
       </c>
@@ -14971,7 +15002,7 @@
         <v>-1.6529605352588106</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="32">
         <v>43880</v>
       </c>
@@ -14986,7 +15017,7 @@
         <v>-1.5917833968562081</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="32">
         <v>43881</v>
       </c>
@@ -15001,7 +15032,7 @@
         <v>-1.5869536022583384</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="32">
         <v>43882</v>
       </c>
@@ -15016,7 +15047,7 @@
         <v>-1.5756390601957304</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="32">
         <v>43885</v>
       </c>
@@ -15031,7 +15062,7 @@
         <v>-1.5726252703963901</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="32">
         <v>43886</v>
       </c>
@@ -15046,7 +15077,7 @@
         <v>-1.5686458442076845</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="32">
         <v>43887</v>
       </c>
@@ -15061,7 +15092,7 @@
         <v>-1.5536633360371053</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="32">
         <v>43888</v>
       </c>
@@ -15076,7 +15107,7 @@
         <v>-1.536219319052825</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" s="32">
         <v>43889</v>
       </c>
@@ -15091,7 +15122,7 @@
         <v>-1.5282068230176424</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="32">
         <v>43892</v>
       </c>
@@ -22122,7 +22153,7 @@
   <dimension ref="A1:Q211"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>